<commit_message>
Generated CE_a results for all reference software and some minor fixes
</commit_message>
<xml_diff>
--- a/input/Analytical-HTAL1/0/Std140_CE_a_Output.xlsx
+++ b/input/Analytical-HTAL1/0/Std140_CE_a_Output.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Analytical-HTAL1\0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C6128CC-E1D1-4127-9275-D0C73307B9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2194233F-202B-4013-8602-4579089835C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="2805" windowWidth="30675" windowHeight="17970" xr2:uid="{A8C11837-0D16-4C14-957E-D1E46740A600}"/>
+    <workbookView xWindow="13545" yWindow="2400" windowWidth="40575" windowHeight="15465" xr2:uid="{A8C11837-0D16-4C14-957E-D1E46740A600}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
   </definedNames>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Program Name and Version (with full build detail):</t>
   </si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>HTAL1 (analytical verification) updated by jn 15 Aug 00 (Markus' results sent 25 Jul 00)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -242,108 +242,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Read Me"/>
-      <sheetName val="Adding Results"/>
-      <sheetName val="YourData"/>
-      <sheetName val="Title Page"/>
-      <sheetName val="Program List"/>
-      <sheetName val="Table List"/>
-      <sheetName val="Figure List"/>
-      <sheetName val="Q-Prt1"/>
-      <sheetName val="Q-Prt2"/>
-      <sheetName val="Q-Prt3"/>
-      <sheetName val="Q-Prt4"/>
-      <sheetName val="Q-Prt5"/>
-      <sheetName val="Q-Prt6"/>
-      <sheetName val="Q-Prt7"/>
-      <sheetName val="Fig B16.5.1-1 COP"/>
-      <sheetName val="Fig B16.5.1-2 COPvar"/>
-      <sheetName val="Fig B16.5.1-3 delCOP"/>
-      <sheetName val="Fig B16.5.1-4 Qtot"/>
-      <sheetName val="Fig B16.5.1-5 dQtot"/>
-      <sheetName val="Fig B16.5.1-6 Qcomp"/>
-      <sheetName val="Fig B16.5.1-7 dQcomp"/>
-      <sheetName val="Fig B16.5.1-8 Qidfan"/>
-      <sheetName val="Fig B16.5.1-9 dQidfan"/>
-      <sheetName val="Fig B16.5.1-10 Qodfan"/>
-      <sheetName val="Fig B16.5.1-11 dQodfan"/>
-      <sheetName val="Fig B16.5.1-12 QCtot"/>
-      <sheetName val="Fig B16.5.1-13 dQCtot"/>
-      <sheetName val="Fig B16.5.1-14 QCsens"/>
-      <sheetName val="Fig B16.5.1-15 dQCsens"/>
-      <sheetName val="Fig B16.5.1-16 QClat"/>
-      <sheetName val="Fig B16.5.1-17 dQClat"/>
-      <sheetName val="Fig B16.5.1-18 IDB"/>
-      <sheetName val="Fig B16.5.1-19 IDBvar"/>
-      <sheetName val="Fig B16.5.1-20 Humrat"/>
-      <sheetName val="Fig B16.5.1-21 Humratvar"/>
-      <sheetName val="Fig B16.5.1-22 QZtot"/>
-      <sheetName val="Fig B16.5.1-23 QZsens"/>
-      <sheetName val="Fig B16.5.1-24 QZlat"/>
-      <sheetName val="Fig B16.5.1-25 Qfan"/>
-      <sheetName val="Fig B16.5.1-26 QCL-QZL"/>
-      <sheetName val="A"/>
-      <sheetName val="Q"/>
-      <sheetName val="Data-Electr"/>
-      <sheetName val="Data-COP"/>
-      <sheetName val="Data-Loads"/>
-      <sheetName val="Data-Delta"/>
-      <sheetName val="Data-TempHum"/>
-      <sheetName val="DOE21E-NREL"/>
-      <sheetName val="DOE21E-CIEMAT"/>
-      <sheetName val="CLM2000"/>
-      <sheetName val="TRN-id"/>
-      <sheetName val="TRN-re"/>
-      <sheetName val="CA-SIS"/>
-      <sheetName val="E+V1"/>
-      <sheetName val="Analytical-TUD"/>
-      <sheetName val="Analytical-HTAL1"/>
-      <sheetName val="Analytical-HTAL2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,9 +561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB23DCD-8829-4965-B4F6-86579D29C695}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V26" sqref="V26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -755,12 +655,12 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75">
+    <row r="23" spans="1:22" ht="15.75">
       <c r="A23" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:22">
       <c r="A25">
         <v>100</v>
       </c>
@@ -803,8 +703,11 @@
       <c r="N25">
         <v>7.3400000000000002E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="V25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26">
         <v>110</v>
       </c>
@@ -848,7 +751,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:22">
       <c r="A27">
         <v>120</v>
       </c>
@@ -892,7 +795,7 @@
         <v>7.8600000000000007E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:22">
       <c r="A28">
         <v>130</v>
       </c>
@@ -936,7 +839,7 @@
         <v>7.3400000000000002E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:22">
       <c r="A29">
         <v>140</v>
       </c>
@@ -980,7 +883,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:22">
       <c r="A30">
         <v>150</v>
       </c>
@@ -1024,7 +927,7 @@
         <v>8.2000000000000007E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:22">
       <c r="A31">
         <v>160</v>
       </c>
@@ -1068,7 +971,7 @@
         <v>9.9399999999999992E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:22">
       <c r="A32">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
First CE_a table working and all that entails
</commit_message>
<xml_diff>
--- a/input/Analytical-HTAL1/0/Std140_CE_a_Output.xlsx
+++ b/input/Analytical-HTAL1/0/Std140_CE_a_Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\JasonGlazer--ashrae-140-automation\input\Analytical-HTAL1\0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2194233F-202B-4013-8602-4579089835C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D010467D-A2DF-47C2-AA81-A953ECB9E969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="2400" windowWidth="40575" windowHeight="15465" xr2:uid="{A8C11837-0D16-4C14-957E-D1E46740A600}"/>
+    <workbookView xWindow="4335" yWindow="3180" windowWidth="26715" windowHeight="15465" xr2:uid="{A8C11837-0D16-4C14-957E-D1E46740A600}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Program Name and Version (with full build detail):</t>
   </si>
@@ -75,6 +75,48 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>CE100</t>
+  </si>
+  <si>
+    <t>CE110</t>
+  </si>
+  <si>
+    <t>CE120</t>
+  </si>
+  <si>
+    <t>CE130</t>
+  </si>
+  <si>
+    <t>CE140</t>
+  </si>
+  <si>
+    <t>CE150</t>
+  </si>
+  <si>
+    <t>CE160</t>
+  </si>
+  <si>
+    <t>CE165</t>
+  </si>
+  <si>
+    <t>CE170</t>
+  </si>
+  <si>
+    <t>CE180</t>
+  </si>
+  <si>
+    <t>CE185</t>
+  </si>
+  <si>
+    <t>CE190</t>
+  </si>
+  <si>
+    <t>CE195</t>
+  </si>
+  <si>
+    <t>CE200</t>
   </si>
 </sst>
 </file>
@@ -563,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB23DCD-8829-4965-B4F6-86579D29C695}">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,8 +703,8 @@
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25">
-        <v>100</v>
+      <c r="A25" t="s">
+        <v>12</v>
       </c>
       <c r="B25">
         <v>1530.8</v>
@@ -708,8 +750,8 @@
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26">
-        <v>110</v>
+      <c r="A26" t="s">
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1077.2</v>
@@ -752,8 +794,8 @@
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27">
-        <v>120</v>
+      <c r="A27" t="s">
+        <v>14</v>
       </c>
       <c r="B27">
         <v>1011</v>
@@ -796,8 +838,8 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28">
-        <v>130</v>
+      <c r="A28" t="s">
+        <v>15</v>
       </c>
       <c r="B28">
         <v>109.5</v>
@@ -840,8 +882,8 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29">
-        <v>140</v>
+      <c r="A29" t="s">
+        <v>16</v>
       </c>
       <c r="B29">
         <v>68.5</v>
@@ -884,8 +926,8 @@
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30">
-        <v>150</v>
+      <c r="A30" t="s">
+        <v>17</v>
       </c>
       <c r="B30">
         <v>1206.5</v>
@@ -928,8 +970,8 @@
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31">
-        <v>160</v>
+      <c r="A31" t="s">
+        <v>18</v>
       </c>
       <c r="B31">
         <v>1139.3</v>
@@ -972,8 +1014,8 @@
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32">
-        <v>165</v>
+      <c r="A32" t="s">
+        <v>19</v>
       </c>
       <c r="B32">
         <v>1499.7</v>
@@ -1016,8 +1058,8 @@
       </c>
     </row>
     <row r="33" spans="1:14">
-      <c r="A33">
-        <v>170</v>
+      <c r="A33" t="s">
+        <v>20</v>
       </c>
       <c r="B33">
         <v>637.70000000000005</v>
@@ -1060,8 +1102,8 @@
       </c>
     </row>
     <row r="34" spans="1:14">
-      <c r="A34">
-        <v>180</v>
+      <c r="A34" t="s">
+        <v>21</v>
       </c>
       <c r="B34">
         <v>1082.3</v>
@@ -1104,8 +1146,8 @@
       </c>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35">
-        <v>185</v>
+      <c r="A35" t="s">
+        <v>22</v>
       </c>
       <c r="B35">
         <v>1543.4</v>
@@ -1148,8 +1190,8 @@
       </c>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36">
-        <v>190</v>
+      <c r="A36" t="s">
+        <v>23</v>
       </c>
       <c r="B36">
         <v>164.1</v>
@@ -1192,8 +1234,8 @@
       </c>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37">
-        <v>195</v>
+      <c r="A37" t="s">
+        <v>24</v>
       </c>
       <c r="B37">
         <v>250</v>
@@ -1236,8 +1278,8 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38">
-        <v>200</v>
+      <c r="A38" t="s">
+        <v>25</v>
       </c>
       <c r="B38">
         <v>1477.4</v>

</xml_diff>